<commit_message>
READy excercise html website
</commit_message>
<xml_diff>
--- a/data/raw-data/exampledata2.xlsx
+++ b/data/raw-data/exampledata2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CE1CF87-64A8-4121-A119-F459E859C75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D57A1E6-7386-496E-996F-9C56019794E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -433,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -700,14 +700,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="35.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>